<commit_message>
feat: designed new dashboard to fit with the project
</commit_message>
<xml_diff>
--- a/public/assets/docs/Format Daftar NIT - Sistem Pembayaran Wira Bahari.xlsx
+++ b/public/assets/docs/Format Daftar NIT - Sistem Pembayaran Wira Bahari.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FAYKAR\15 Projects\SMK Wira Bahari\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FAYKAR\15 Projects\SMK Wira Bahari\wira-pay\public\assets\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D4CDA5-09B2-476E-9977-A0EC5B9D48CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4702350-A993-4251-8F97-05CE02AD6B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2BB23C2A-04CD-4721-B8EC-6D980212C6A3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>NIT</t>
   </si>
@@ -36,14 +36,26 @@
     <t>20.22.254</t>
   </si>
   <si>
-    <t>CONTOH NAMA</t>
+    <t>DAFTAR NIT SISWA SMK WIRA BAHARI</t>
+  </si>
+  <si>
+    <t>TAHUN AKADEMIK 2025/2026</t>
+  </si>
+  <si>
+    <t>Downloaded From : Sistem Pembayaran Siswa Baru SMK Wira Bahari</t>
+  </si>
+  <si>
+    <t>Contoh Nama Lengkap</t>
+  </si>
+  <si>
+    <t>JURUSAN : NKPI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,6 +72,19 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Book Antiqua"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Book Antiqua"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Book Antiqua"/>
       <family val="1"/>
@@ -100,11 +125,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,36 +459,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB1CA41-09A4-4568-A788-177D04143981}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C2" sqref="C2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="12" style="8" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
+      <c r="B5" s="8" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C2:H2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: deleted jurusan CRUD & the table
</commit_message>
<xml_diff>
--- a/public/assets/docs/Format Daftar NIT - Sistem Pembayaran Wira Bahari.xlsx
+++ b/public/assets/docs/Format Daftar NIT - Sistem Pembayaran Wira Bahari.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FAYKAR\15 Projects\SMK Wira Bahari\wira-pay\public\assets\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4702350-A993-4251-8F97-05CE02AD6B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF425A1A-786E-478E-9189-8C87E214977D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2BB23C2A-04CD-4721-B8EC-6D980212C6A3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>NIT</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Contoh Nama Lengkap</t>
-  </si>
-  <si>
-    <t>JURUSAN : NKPI</t>
   </si>
 </sst>
 </file>
@@ -125,25 +122,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -459,73 +452,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB1CA41-09A4-4568-A788-177D04143981}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:H2"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12" style="8" customWidth="1"/>
-    <col min="2" max="2" width="45.28515625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="12" style="4" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" style="4" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="2"/>
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
     <mergeCell ref="C2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: create a view for history transaksi pembayaran with dynamic data
</commit_message>
<xml_diff>
--- a/public/assets/docs/Format Daftar NIT - Sistem Pembayaran Wira Bahari.xlsx
+++ b/public/assets/docs/Format Daftar NIT - Sistem Pembayaran Wira Bahari.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FAYKAR\15 Projects\SMK Wira Bahari\wira-pay\public\assets\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF425A1A-786E-478E-9189-8C87E214977D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213A9B30-90E5-4FF5-99E4-877AB9163A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2BB23C2A-04CD-4721-B8EC-6D980212C6A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{2BB23C2A-04CD-4721-B8EC-6D980212C6A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,13 +39,13 @@
     <t>DAFTAR NIT SISWA SMK WIRA BAHARI</t>
   </si>
   <si>
-    <t>TAHUN AKADEMIK 2025/2026</t>
-  </si>
-  <si>
-    <t>Downloaded From : Sistem Pembayaran Siswa Baru SMK Wira Bahari</t>
-  </si>
-  <si>
     <t>Contoh Nama Lengkap</t>
+  </si>
+  <si>
+    <t>Downloaded From : Sistem Pembayaran Siswa SMK Wira Bahari</t>
+  </si>
+  <si>
+    <t>TAHUN AKADEMIK 20XX/20XX</t>
   </si>
 </sst>
 </file>
@@ -136,7 +136,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,7 +477,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -502,7 +502,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>